<commit_message>
angular tutorials + sprint 1
Trying out some things with chart format
Beginning of angular tutorial
</commit_message>
<xml_diff>
--- a/Week 3/HoursPerWeek.xlsx
+++ b/Week 3/HoursPerWeek.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\Documents\GitKraken\CITS3200Research\Week 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\Documents\GitKraken\CITS3200Research\Week 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Week</t>
   </si>
@@ -61,12 +61,21 @@
   <si>
     <t>Ruby</t>
   </si>
+  <si>
+    <t>Ruben</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,13 +83,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -92,13 +137,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -135,25 +190,21 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-AU"/>
-              <a:t>Avaliable Hours</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> per Week</a:t>
+              <a:t>Avaliable Hours per Week</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -167,6 +218,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -190,9 +261,71 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:schemeClr val="accent3"/>
             </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
           </c:spPr>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$13</c:f>
@@ -304,9 +437,71 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:schemeClr val="accent5"/>
             </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
           </c:spPr>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$13</c:f>
@@ -358,9 +553,141 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ruben</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-75E4-4466-BAE9-7F803D74EFE1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -380,7 +707,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -398,9 +725,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -412,9 +739,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -445,7 +772,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -463,9 +790,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -479,7 +806,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -496,11 +823,75 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -540,25 +931,21 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-AU"/>
-              <a:t>Avaliable Hours</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> per Week</a:t>
+              <a:t>Avaliable Hours per Week</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -572,6 +959,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -596,8 +1003,12 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:schemeClr val="accent3"/>
             </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -711,8 +1122,12 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:schemeClr val="accent5"/>
             </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
@@ -763,6 +1178,81 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-D498-43A1-A54F-4BE9B8328799}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ruben</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-64CF-4DC2-8050-20D9482612BB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -774,7 +1264,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="267"/>
+        <c:overlap val="-43"/>
         <c:axId val="1933511408"/>
         <c:axId val="1933501840"/>
       </c:barChart>
@@ -789,7 +1280,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -807,9 +1298,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -821,9 +1312,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -854,7 +1345,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -870,14 +1361,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -888,7 +1373,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -905,11 +1390,75 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -928,18 +1477,2382 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Experience/Confidence Level</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.6580927384076991E-2"/>
+          <c:y val="0.17171296296296298"/>
+          <c:w val="0.90286351706036749"/>
+          <c:h val="0.61498432487605714"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Evan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$18:$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Java</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Python</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>JavaScript</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SQL</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>PHP</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ruby</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ADBD-49BC-960C-AAE80D130FE4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Janice</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$18:$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Java</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Python</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>JavaScript</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SQL</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>PHP</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ruby</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$18:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ADBD-49BC-960C-AAE80D130FE4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ruben</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$18:$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Java</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Python</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>JavaScript</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SQL</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>PHP</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ruby</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$18:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-ADBD-49BC-960C-AAE80D130FE4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="267"/>
+        <c:overlap val="-43"/>
+        <c:axId val="132618752"/>
+        <c:axId val="132615424"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="132618752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="132615424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="132615424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="132618752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="282">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="208">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="208">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>11767</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>516031</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>89086</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>598956</xdr:colOff>
+      <xdr:colOff>554132</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>41462</xdr:rowOff>
     </xdr:to>
@@ -962,16 +3875,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>22411</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>537881</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>56028</xdr:rowOff>
+      <xdr:rowOff>156880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>4482</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>8404</xdr:rowOff>
+      <xdr:rowOff>109256</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -987,6 +3900,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>504266</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>40341</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>291354</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>116541</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1258,10 +4201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,7 +4213,7 @@
     <col min="13" max="13" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1280,8 +4223,17 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1291,8 +4243,19 @@
       <c r="C2">
         <v>2</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <f>AVERAGE(B2:F2)</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="J2" s="3">
+        <f>SUM(B2:F2)</f>
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1302,8 +4265,19 @@
       <c r="C3">
         <v>4</v>
       </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I13" si="0">AVERAGE(B3:F3)</f>
+        <v>4</v>
+      </c>
+      <c r="J3" s="4">
+        <f t="shared" ref="J3:J13" si="1">SUM(B3:F3)</f>
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1313,8 +4287,19 @@
       <c r="C4">
         <v>6</v>
       </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="0"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1324,8 +4309,19 @@
       <c r="C5">
         <v>10</v>
       </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1335,8 +4331,19 @@
       <c r="C6">
         <v>6</v>
       </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1346,8 +4353,19 @@
       <c r="C7">
         <v>6</v>
       </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1357,8 +4375,19 @@
       <c r="C8">
         <v>4</v>
       </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1368,8 +4397,19 @@
       <c r="C9">
         <v>3</v>
       </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1379,8 +4419,19 @@
       <c r="C10">
         <v>10</v>
       </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1390,8 +4441,19 @@
       <c r="C11">
         <v>4</v>
       </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1401,8 +4463,19 @@
       <c r="C12">
         <v>6</v>
       </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1412,8 +4485,19 @@
       <c r="C13">
         <v>5</v>
       </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1425,8 +4509,26 @@
         <f>SUM(C4:C13)</f>
         <v>60</v>
       </c>
+      <c r="D15">
+        <f>SUM(D2:D13)</f>
+        <v>60</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1436,8 +4538,15 @@
       <c r="C18">
         <v>8</v>
       </c>
+      <c r="D18">
+        <v>9</v>
+      </c>
+      <c r="I18">
+        <f>AVERAGE(B18:D18)</f>
+        <v>8.6666666666666661</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1447,8 +4556,15 @@
       <c r="C19">
         <v>7</v>
       </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <f>AVERAGE(B19:D19)</f>
+        <v>5.333333333333333</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1458,8 +4574,15 @@
       <c r="C20">
         <v>7</v>
       </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="I20">
+        <f>AVERAGE(B20:D20)</f>
+        <v>6.333333333333333</v>
+      </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1469,8 +4592,15 @@
       <c r="C21">
         <v>8</v>
       </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <f>AVERAGE(B21:D21)</f>
+        <v>4</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1480,8 +4610,15 @@
       <c r="C22">
         <v>8</v>
       </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <f>AVERAGE(B22:D22)</f>
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1491,8 +4628,15 @@
       <c r="C23">
         <v>1</v>
       </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <f>AVERAGE(B23:D23)</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1500,6 +4644,13 @@
         <v>1</v>
       </c>
       <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <f>AVERAGE(B24:D24)</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sprint 1 + Angular
Added Jess data/random angular snippets
</commit_message>
<xml_diff>
--- a/Week 3/HoursPerWeek.xlsx
+++ b/Week 3/HoursPerWeek.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Week</t>
   </si>
@@ -69,6 +69,24 @@
   </si>
   <si>
     <t>SUM</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Jess</t>
+  </si>
+  <si>
+    <t>Part-Time</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Git</t>
   </si>
 </sst>
 </file>
@@ -682,6 +700,141 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-75E4-4466-BAE9-7F803D74EFE1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Jess</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1818-4700-99F2-7CB785E9C97C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1253,6 +1406,84 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-64CF-4DC2-8050-20D9482612BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Jess</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B50D-4B6F-AD5A-A529DED612C1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1590,9 +1821,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$18:$A$24</c:f>
+              <c:f>Sheet1!$A$18:$A$25</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Java</c:v>
                 </c:pt>
@@ -1613,16 +1844,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Ruby</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Git</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$18:$B$24</c:f>
+              <c:f>Sheet1!$B$18:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>9</c:v>
                 </c:pt>
@@ -1633,7 +1867,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3</c:v>
@@ -1643,6 +1877,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1679,9 +1916,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$18:$A$24</c:f>
+              <c:f>Sheet1!$A$18:$A$25</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Java</c:v>
                 </c:pt>
@@ -1702,16 +1939,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Ruby</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Git</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$24</c:f>
+              <c:f>Sheet1!$C$18:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>8</c:v>
                 </c:pt>
@@ -1732,6 +1972,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1768,9 +2011,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$18:$A$24</c:f>
+              <c:f>Sheet1!$A$18:$A$25</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Java</c:v>
                 </c:pt>
@@ -1791,16 +2034,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Ruby</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Git</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$18:$D$24</c:f>
+              <c:f>Sheet1!$D$18:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>9</c:v>
                 </c:pt>
@@ -1820,6 +2066,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1828,6 +2077,101 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-ADBD-49BC-960C-AAE80D130FE4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Jess</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$18:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Java</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Python</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>JavaScript</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SQL</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>PHP</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ruby</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Git</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$18:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-49A8-4494-8936-EA2E1144EE71}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3907,16 +4251,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>504266</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>11207</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>40341</xdr:rowOff>
+      <xdr:rowOff>6724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>291354</xdr:colOff>
+      <xdr:colOff>347383</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>116541</xdr:rowOff>
+      <xdr:rowOff>82924</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4201,14 +4545,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="11" max="11" width="7" customWidth="1"/>
     <col min="13" max="13" width="8.28515625" customWidth="1"/>
   </cols>
@@ -4226,6 +4571,12 @@
       <c r="D1" t="s">
         <v>12</v>
       </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
       <c r="I1" t="s">
         <v>13</v>
       </c>
@@ -4246,13 +4597,16 @@
       <c r="D2">
         <v>0</v>
       </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
       <c r="I2" s="1">
-        <f>AVERAGE(B2:F2)</f>
-        <v>1.6666666666666667</v>
+        <f>AVERAGE(A2:E2)</f>
+        <v>1.6</v>
       </c>
       <c r="J2" s="3">
-        <f>SUM(B2:F2)</f>
-        <v>5</v>
+        <f>SUM(A2:E2)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -4268,13 +4622,16 @@
       <c r="D3">
         <v>4</v>
       </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I13" si="0">AVERAGE(B3:F3)</f>
-        <v>4</v>
-      </c>
-      <c r="J3" s="4">
-        <f t="shared" ref="J3:J13" si="1">SUM(B3:F3)</f>
-        <v>12</v>
+        <f t="shared" ref="I3:I13" si="0">AVERAGE(A3:E3)</f>
+        <v>3.6</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" ref="J3:J13" si="1">SUM(A3:E3)</f>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -4290,13 +4647,16 @@
       <c r="D4">
         <v>4</v>
       </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
       <c r="I4" s="1">
         <f t="shared" si="0"/>
-        <v>5.333333333333333</v>
-      </c>
-      <c r="J4" s="4">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J4" s="3">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -4312,13 +4672,16 @@
       <c r="D5">
         <v>4</v>
       </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
-        <v>6.666666666666667</v>
-      </c>
-      <c r="J5" s="2">
+        <v>5.4</v>
+      </c>
+      <c r="J5" s="4">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -4334,13 +4697,16 @@
       <c r="D6">
         <v>2</v>
       </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
       <c r="I6" s="1">
         <f t="shared" si="0"/>
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="J6" s="4">
+        <v>4</v>
+      </c>
+      <c r="J6" s="3">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -4356,13 +4722,16 @@
       <c r="D7">
         <v>5</v>
       </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
-        <v>5.333333333333333</v>
+        <v>5.4</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -4378,13 +4747,16 @@
       <c r="D8">
         <v>5</v>
       </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
-        <v>4.666666666666667</v>
+        <v>5.2</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -4400,13 +4772,16 @@
       <c r="D9">
         <v>6</v>
       </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
-        <v>4.666666666666667</v>
+        <v>5.4</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -4422,13 +4797,16 @@
       <c r="D10">
         <v>10</v>
       </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
       <c r="I10" s="1">
         <f t="shared" si="0"/>
-        <v>9.3333333333333339</v>
+        <v>9.5</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -4444,13 +4822,16 @@
       <c r="D11">
         <v>5</v>
       </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
       <c r="I11" s="1">
         <f t="shared" si="0"/>
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="J11" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="J11" s="4">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -4466,13 +4847,16 @@
       <c r="D12">
         <v>5</v>
       </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
       <c r="I12" s="1">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>7.2</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -4488,13 +4872,16 @@
       <c r="D13">
         <v>10</v>
       </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
       <c r="I13" s="1">
         <f t="shared" si="0"/>
-        <v>8.3333333333333339</v>
+        <v>7.8</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -4513,6 +4900,14 @@
         <f>SUM(D2:D13)</f>
         <v>60</v>
       </c>
+      <c r="E15">
+        <f>SUM(E2:E13)</f>
+        <v>55</v>
+      </c>
+      <c r="F15">
+        <f>SUM(F2:F13)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -4524,6 +4919,12 @@
       <c r="D17" t="s">
         <v>12</v>
       </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
       <c r="I17" t="s">
         <v>13</v>
       </c>
@@ -4541,9 +4942,12 @@
       <c r="D18">
         <v>9</v>
       </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
       <c r="I18">
-        <f>AVERAGE(B18:D18)</f>
-        <v>8.6666666666666661</v>
+        <f>AVERAGE(B18:F18)</f>
+        <v>6.75</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -4559,9 +4963,12 @@
       <c r="D19">
         <v>2</v>
       </c>
+      <c r="E19">
+        <v>8</v>
+      </c>
       <c r="I19">
-        <f>AVERAGE(B19:D19)</f>
-        <v>5.333333333333333</v>
+        <f>AVERAGE(B19:F19)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -4577,9 +4984,12 @@
       <c r="D20">
         <v>8</v>
       </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
       <c r="I20">
-        <f>AVERAGE(B20:D20)</f>
-        <v>6.333333333333333</v>
+        <f>AVERAGE(B20:F20)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -4587,7 +4997,7 @@
         <v>8</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21">
         <v>8</v>
@@ -4595,9 +5005,12 @@
       <c r="D21">
         <v>2</v>
       </c>
+      <c r="E21">
+        <v>7</v>
+      </c>
       <c r="I21">
-        <f>AVERAGE(B21:D21)</f>
-        <v>4</v>
+        <f>AVERAGE(B21:F21)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -4613,9 +5026,12 @@
       <c r="D22">
         <v>1</v>
       </c>
+      <c r="E22">
+        <v>8</v>
+      </c>
       <c r="I22">
-        <f>AVERAGE(B22:D22)</f>
-        <v>4</v>
+        <f>AVERAGE(B22:F22)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -4631,9 +5047,12 @@
       <c r="D23">
         <v>1</v>
       </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
       <c r="I23">
-        <f>AVERAGE(B23:D23)</f>
-        <v>1</v>
+        <f>AVERAGE(B23:F23)</f>
+        <v>1.25</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -4649,9 +5068,53 @@
       <c r="D24">
         <v>1</v>
       </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
       <c r="I24">
-        <f>AVERAGE(B24:D24)</f>
+        <f>AVERAGE(B24:F24)</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>8</v>
+      </c>
+      <c r="I25">
+        <f>AVERAGE(B25:E25)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>